<commit_message>
Data and Graph Update
</commit_message>
<xml_diff>
--- a/final_testData.xlsx
+++ b/final_testData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21810"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F32B6C2-C213-43E2-BD37-D79D552930D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459945DD-A67F-4A9F-83C6-E8564BBCF39D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
   <si>
     <t>Test 1</t>
   </si>
@@ -207,13 +207,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -242,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -260,7 +260,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -339,7 +339,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -407,7 +407,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -561,7 +561,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -678,6 +678,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>First</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t> Version's 10 Missions vs. Improved Version's First 10 Missions</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
@@ -708,7 +768,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="29492655"/>
@@ -739,6 +799,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t> (Seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
@@ -769,7 +889,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="26645103"/>
@@ -811,7 +931,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -848,7 +968,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -862,7 +982,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -903,6 +1023,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.32821992391986926"/>
+          <c:y val="1.5460244164731702E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -928,7 +1056,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -996,7 +1124,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="b"/>
@@ -1150,7 +1278,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1266,6 +1394,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>First Version's 10 Missions vs. Improved Version's First 10 Missions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1299,7 +1482,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="29491407"/>
@@ -1330,6 +1513,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t> (Seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1358,7 +1601,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="284691903"/>
@@ -1400,7 +1643,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1437,7 +1680,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1451,7 +1694,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1511,7 +1754,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> Success Rate</a:t>
+              <a:t> Training Success Rate</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="1">
               <a:solidFill>
@@ -1546,7 +1789,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1628,7 +1871,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="bestFit"/>
@@ -1739,7 +1982,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1776,7 +2019,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1790,7 +2033,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1856,7 +2099,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1938,7 +2181,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="bestFit"/>
@@ -2048,7 +2291,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2085,7 +2328,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2099,7 +2342,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2172,7 +2415,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2224,7 +2467,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -2359,6 +2602,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Mission</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t> #</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2393,7 +2696,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1124569136"/>
@@ -2407,6 +2710,7 @@
         <c:axId val="1124569136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2424,6 +2728,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Time (Seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2452,7 +2812,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="817568672"/>
@@ -2493,7 +2853,529 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Agent Travel Time</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00_);[Red]\(#,##0.00\)" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$H$7:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$7:$L$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.2534370422363201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.90856480598449</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0422346591949401</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2444312572479204</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.71627473831176</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9275028705596902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3190548419952299</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.9262206554412802</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.66298127174377</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.8523998260498002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FC72-47AE-9E25-9A434922511B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1751297471"/>
+        <c:axId val="1458408943"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1751297471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Mission</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t> #</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1458408943"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1458408943"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t> (Seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1751297471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2704,6 +3586,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -4749,6 +5671,509 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5433,6 +6858,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>89203</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>20768</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>943328</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>7516</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="图表 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80EF9565-D76A-4A5F-8C38-42B59C417514}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5702,16 +7163,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AZ56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="X42" sqref="X42"/>
+    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">

</xml_diff>